<commit_message>
Extracting Feature with Noise Augmented
</commit_message>
<xml_diff>
--- a/exp/2022/Logbook_Eksperiment.xlsx
+++ b/exp/2022/Logbook_Eksperiment.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7770" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7770" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Conf-1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="250">
   <si>
     <t>Tanggal</t>
   </si>
@@ -726,6 +726,66 @@
   </si>
   <si>
     <t>exp-9_2</t>
+  </si>
+  <si>
+    <t>Epoch 200, tanpa dropout 0.5, Noise_augment</t>
+  </si>
+  <si>
+    <t>exp-10_1</t>
+  </si>
+  <si>
+    <t>Epoch 200, dropout 0.5, Noise_augment</t>
+  </si>
+  <si>
+    <t>exp-10_2</t>
+  </si>
+  <si>
+    <t>exp-10_3</t>
+  </si>
+  <si>
+    <t>exp-10_4</t>
+  </si>
+  <si>
+    <t>exp-10_5</t>
+  </si>
+  <si>
+    <t>exp-10_6</t>
+  </si>
+  <si>
+    <t>exp-10_7</t>
+  </si>
+  <si>
+    <t>exp-10_8</t>
+  </si>
+  <si>
+    <t>exp-11_1</t>
+  </si>
+  <si>
+    <t>Epoch 200, tanpa dropout 0.5, Noise_augment, MinMaxScaler per Audio</t>
+  </si>
+  <si>
+    <t>Epoch 200, dropout 0.5, Noise_augment, MinMaxScaler per Audio</t>
+  </si>
+  <si>
+    <t>exp-11_2</t>
+  </si>
+  <si>
+    <t>exp-11_3</t>
+  </si>
+  <si>
+    <t>exp-11_4</t>
+  </si>
+  <si>
+    <t>exp-11_5</t>
+  </si>
+  <si>
+    <t>exp-11_6</t>
+  </si>
+  <si>
+    <t>exp-11_7</t>
+  </si>
+  <si>
+    <t>exp-11_8</t>
   </si>
 </sst>
 </file>
@@ -3918,10 +3978,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F78"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A78" sqref="A78"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5492,6 +5552,326 @@
       </c>
       <c r="F78" s="3" t="s">
         <v>229</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D79" s="3">
+        <v>55.71</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D80" s="3">
+        <v>63.31</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D81" s="3">
+        <v>66.489999999999995</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D82" s="3">
+        <v>61.43</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D83" s="3">
+        <v>61.04</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D84" s="3">
+        <v>62.22</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" s="3">
+        <v>65.58</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D86" s="3">
+        <v>59.98</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D87" s="3">
+        <v>62.22</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D88" s="3">
+        <v>59.56</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D89" s="3">
+        <v>68.34</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D90" s="3">
+        <v>64.2</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D91" s="3">
+        <v>68.34</v>
+      </c>
+      <c r="E91" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D92" s="3">
+        <v>64.2</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D93" s="3">
+        <v>62.42</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>44606</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D94" s="3">
+        <v>61.53</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -5649,15 +6029,15 @@
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E32C6C59-7111-4FF1-B57C-8954CAF8C697}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f64f122a-13cb-4691-a415-cbf7b0e63df3"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>